<commit_message>
Løst oppgave 1, 3 og 4. Nesten ferdig med 2 også, men mangler litt. Overskriver eksisterende, siden det var kommet så kort før en nå merge prosess, så erstatning er like greit.
</commit_message>
<xml_diff>
--- a/barnehage/kgdata.xlsx
+++ b/barnehage/kgdata.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:F1"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,6 +461,334 @@
         <is>
           <t>foresatt_pnr</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>12</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>11</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Reidar</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Adressesvingen 7</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>45454545</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>04048701234</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>10</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Tormund</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Postboks 5</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>48544646</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>20018500100</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>9</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Finn</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Postboks 5</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>47474747</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>10108020301</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>8</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Filip</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Hammeren 106</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>45282401</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>15029165444</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>7</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Cathrine</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Hammeren 106</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>95793421</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>12048952153</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Janne</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Grevlingstien 44</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>47432211</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>15119165456</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>5</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Selma</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Grevlingstien 44</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>43643522</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>27048932123</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Katrine</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Svingen 10</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>45452323</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>01019500100</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Rebecca</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Tiurveien 12</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>99778866</v>
+      </c>
+      <c r="F12" t="n">
+        <v>30109243533</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Kristoffer</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Tiurveien 12</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>99887766</v>
+      </c>
+      <c r="F13" t="n">
+        <v>15029022422</v>
       </c>
     </row>
   </sheetData>
@@ -648,7 +976,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:C1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -666,6 +994,74 @@
         <is>
           <t>barn_pnr</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>17052143210</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>31012344544</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" t="n">
+        <v>30062174510</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>12122278987</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2032290301</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>4042011411</v>
       </c>
     </row>
   </sheetData>
@@ -679,7 +1075,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:M1"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -749,6 +1145,226 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C2" t="n">
+        <v>11</v>
+      </c>
+      <c r="D2" t="n">
+        <v>12</v>
+      </c>
+      <c r="E2" t="n">
+        <v>6</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Giggles and Grins Childcare</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>2024-12-23</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>9</v>
+      </c>
+      <c r="D3" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Giggles and Grins Childcare</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>2024-12-23</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D4" t="n">
+        <v>8</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>123 Learning Center</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>2024-12-16</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
+        <v>1200000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Sunshine Preschool</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>2024-12-16</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
+        <v>850000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>ABC Kindergarten</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>2024-12-16</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Sunshine Preschool</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>2024-12-16</t>
+        </is>
+      </c>
+      <c r="M7" t="n">
+        <v>1000000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>